<commit_message>
Update for Generate FW list
</commit_message>
<xml_diff>
--- a/Ultities/Templates/DBCGen_V1_01_od.xlsx
+++ b/Ultities/Templates/DBCGen_V1_01_od.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CANMatrix!$A$1:$AC$224</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="623">
   <si>
     <t>IC_2</t>
   </si>
@@ -2246,6 +2246,24 @@
   </si>
   <si>
     <t>EMS_AccelPedalPosInvalid</t>
+  </si>
+  <si>
+    <t>DNCIF</t>
+  </si>
+  <si>
+    <t>NMSG_MotRpm_UW</t>
+  </si>
+  <si>
+    <t>NMSG_MMotActLm_SW</t>
+  </si>
+  <si>
+    <t>NMSG_Sas_ST.Mode_UB</t>
+  </si>
+  <si>
+    <t>NMSG_MDriverRequest_SW Scl_MDriverRequest_InvalidValue dsadsadsa</t>
+  </si>
+  <si>
+    <t>NMSG_MotPedalPosThrottleValve_UB</t>
   </si>
 </sst>
 </file>
@@ -2267,7 +2285,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2313,6 +2331,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2424,7 +2454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -2484,6 +2514,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2533,7 +2573,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -3229,34 +3289,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="22" t="s">
         <v>602</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="23"/>
+      <c r="E1" s="22" t="s">
         <v>603</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="20"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3266,17 +3326,17 @@
       <c r="C4" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="28" t="s">
         <v>612</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
@@ -3285,15 +3345,15 @@
       <c r="C5" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="33"/>
     </row>
     <row r="6" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -3302,15 +3362,15 @@
       <c r="C6" s="9" t="s">
         <v>591</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="33"/>
     </row>
     <row r="7" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -3319,15 +3379,15 @@
       <c r="C7" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
     </row>
     <row r="8" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
@@ -3336,15 +3396,15 @@
       <c r="C8" s="9" t="s">
         <v>593</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="33"/>
     </row>
     <row r="9" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
@@ -3353,15 +3413,15 @@
       <c r="C9" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
     </row>
     <row r="10" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
@@ -3370,15 +3430,15 @@
       <c r="C10" s="9" t="s">
         <v>594</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -3387,15 +3447,15 @@
       <c r="C11" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -3404,15 +3464,15 @@
       <c r="C12" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -3421,15 +3481,15 @@
       <c r="C13" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="33"/>
     </row>
     <row r="14" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
@@ -3438,15 +3498,15 @@
       <c r="C14" s="9" t="s">
         <v>598</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
     </row>
     <row r="15" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
@@ -3455,15 +3515,15 @@
       <c r="C15" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
@@ -3472,15 +3532,15 @@
       <c r="C16" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
     </row>
     <row r="17" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
@@ -3489,15 +3549,15 @@
       <c r="C17" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
@@ -3506,15 +3566,15 @@
       <c r="C18" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
@@ -3523,15 +3583,15 @@
       <c r="C19" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
@@ -3540,15 +3600,15 @@
       <c r="C20" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="30"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="33"/>
     </row>
     <row r="21" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
@@ -3557,15 +3617,15 @@
       <c r="C21" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
@@ -3574,15 +3634,15 @@
       <c r="C22" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
@@ -3591,15 +3651,15 @@
       <c r="C23" s="9" t="s">
         <v>600</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33"/>
     </row>
     <row r="24" spans="2:13" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
@@ -3608,15 +3668,15 @@
       <c r="C24" s="9" t="s">
         <v>601</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
     </row>
     <row r="25" spans="2:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
@@ -3625,15 +3685,15 @@
       <c r="C25" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="33"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
     </row>
   </sheetData>
   <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1"/>
@@ -3643,10 +3703,10 @@
     <mergeCell ref="E4:M25"/>
   </mergeCells>
   <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"r"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3690,10 +3750,10 @@
   <dimension ref="A1:AS224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A221" sqref="A221"/>
+      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3712,7 +3772,8 @@
     <col min="20" max="20" width="9.140625" style="15"/>
     <col min="21" max="21" width="15" style="15" customWidth="1"/>
     <col min="22" max="29" width="9.140625" style="18"/>
-    <col min="30" max="45" width="9.140625" style="15"/>
+    <col min="30" max="30" width="22.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="45" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -3803,7 +3864,9 @@
       <c r="AC1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="17"/>
+      <c r="AD1" s="19" t="s">
+        <v>617</v>
+      </c>
       <c r="AE1" s="17"/>
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
@@ -3868,6 +3931,7 @@
       </c>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
+      <c r="AD2" s="20"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -3935,6 +3999,9 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
+      <c r="AD3" s="20" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -4002,6 +4069,9 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
+      <c r="AD4" s="21" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -4069,6 +4139,9 @@
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
+      <c r="AD5" s="21" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -4138,6 +4211,7 @@
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
+      <c r="AD6" s="20"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -4205,6 +4279,7 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
+      <c r="AD7" s="20"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -4270,6 +4345,7 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
+      <c r="AD8" s="20"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
@@ -4335,6 +4411,7 @@
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
+      <c r="AD9" s="20"/>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -4400,6 +4477,7 @@
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
+      <c r="AD10" s="20"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -4467,6 +4545,9 @@
       </c>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
+      <c r="AD11" s="20" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
@@ -4532,6 +4613,7 @@
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
+      <c r="AD12" s="20"/>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -4595,6 +4677,7 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
+      <c r="AD13" s="20"/>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -4660,6 +4743,7 @@
       </c>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
+      <c r="AD14" s="20"/>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
@@ -4725,6 +4809,7 @@
       </c>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
+      <c r="AD15" s="20"/>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -4776,8 +4861,9 @@
         <v>11</v>
       </c>
       <c r="AC16" s="5"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD16" s="20"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -4841,8 +4927,9 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD17" s="20"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4912,8 +4999,9 @@
         <v>11</v>
       </c>
       <c r="AC18" s="5"/>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD18" s="20"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -4975,8 +5063,9 @@
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD19" s="20"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -5044,8 +5133,9 @@
         <v>11</v>
       </c>
       <c r="AC20" s="5"/>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD20" s="20"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5109,8 +5199,9 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD21" s="20"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -5176,8 +5267,9 @@
         <v>11</v>
       </c>
       <c r="AC22" s="5"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD22" s="20"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -5243,8 +5335,9 @@
         <v>11</v>
       </c>
       <c r="AC23" s="5"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD23" s="20"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>83</v>
       </c>
@@ -5296,8 +5389,9 @@
         <v>11</v>
       </c>
       <c r="AC24" s="5"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD24" s="20"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -5367,8 +5461,11 @@
       </c>
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD25" s="20" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -5436,8 +5533,9 @@
       </c>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD26" s="20"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -5509,8 +5607,9 @@
         <v>11</v>
       </c>
       <c r="AC27" s="5"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD27" s="20"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -5576,8 +5675,9 @@
       </c>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD28" s="20"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -5643,8 +5743,9 @@
       </c>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD29" s="20"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -5714,8 +5815,9 @@
         <v>11</v>
       </c>
       <c r="AC30" s="5"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD30" s="20"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -5779,8 +5881,9 @@
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD31" s="20"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -5844,8 +5947,9 @@
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD32" s="20"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -5911,8 +6015,9 @@
       </c>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD33" s="20"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -5978,8 +6083,9 @@
       </c>
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD34" s="20"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
@@ -6029,8 +6135,9 @@
       </c>
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD35" s="20"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -6094,8 +6201,9 @@
       <c r="AA36" s="5"/>
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD36" s="20"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -6161,8 +6269,9 @@
       </c>
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD37" s="20"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>118</v>
       </c>
@@ -6214,8 +6323,9 @@
         <v>11</v>
       </c>
       <c r="AC38" s="5"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD38" s="20"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -6279,8 +6389,9 @@
       </c>
       <c r="AB39" s="5"/>
       <c r="AC39" s="5"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD39" s="20"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -6350,8 +6461,9 @@
         <v>11</v>
       </c>
       <c r="AC40" s="5"/>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD40" s="20"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -6421,8 +6533,9 @@
         <v>11</v>
       </c>
       <c r="AC41" s="5"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD41" s="20"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -6494,8 +6607,9 @@
         <v>11</v>
       </c>
       <c r="AC42" s="5"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD42" s="20"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -6563,8 +6677,9 @@
       </c>
       <c r="AB43" s="5"/>
       <c r="AC43" s="5"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD43" s="20"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -6626,8 +6741,9 @@
       <c r="AA44" s="5"/>
       <c r="AB44" s="5"/>
       <c r="AC44" s="5"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD44" s="20"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -6687,8 +6803,9 @@
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
       <c r="AC45" s="5"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD45" s="20"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -6748,8 +6865,9 @@
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
       <c r="AC46" s="5"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD46" s="20"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -6817,8 +6935,9 @@
         <v>11</v>
       </c>
       <c r="AC47" s="5"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD47" s="20"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -6886,8 +7005,9 @@
         <v>11</v>
       </c>
       <c r="AC48" s="5"/>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD48" s="20"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>142</v>
       </c>
@@ -6939,8 +7059,9 @@
         <v>11</v>
       </c>
       <c r="AC49" s="5"/>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD49" s="20"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -7012,8 +7133,9 @@
         <v>11</v>
       </c>
       <c r="AC50" s="5"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD50" s="20"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -7083,8 +7205,9 @@
         <v>11</v>
       </c>
       <c r="AC51" s="5"/>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD51" s="20"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -7148,8 +7271,9 @@
       </c>
       <c r="AB52" s="5"/>
       <c r="AC52" s="5"/>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD52" s="20"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -7221,8 +7345,9 @@
         <v>11</v>
       </c>
       <c r="AC53" s="5"/>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD53" s="20"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -7292,8 +7417,9 @@
         <v>11</v>
       </c>
       <c r="AC54" s="5"/>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD54" s="20"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -7357,8 +7483,9 @@
       </c>
       <c r="AB55" s="5"/>
       <c r="AC55" s="5"/>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD55" s="20"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -7426,8 +7553,9 @@
         <v>11</v>
       </c>
       <c r="AC56" s="5"/>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD56" s="20"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -7495,8 +7623,9 @@
         <v>11</v>
       </c>
       <c r="AC57" s="5"/>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD57" s="20"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -7564,8 +7693,9 @@
         <v>11</v>
       </c>
       <c r="AC58" s="5"/>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD58" s="20"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -7633,8 +7763,9 @@
         <v>11</v>
       </c>
       <c r="AC59" s="5"/>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD59" s="20"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>165</v>
       </c>
@@ -7686,8 +7817,9 @@
         <v>11</v>
       </c>
       <c r="AC60" s="5"/>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD60" s="20"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -7759,8 +7891,9 @@
         <v>11</v>
       </c>
       <c r="AC61" s="5"/>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD61" s="20"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -7830,8 +7963,9 @@
         <v>11</v>
       </c>
       <c r="AC62" s="5"/>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD62" s="20"/>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -7895,8 +8029,9 @@
       </c>
       <c r="AB63" s="5"/>
       <c r="AC63" s="5"/>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD63" s="20"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -7968,8 +8103,9 @@
         <v>11</v>
       </c>
       <c r="AC64" s="5"/>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD64" s="20"/>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -8039,8 +8175,9 @@
         <v>11</v>
       </c>
       <c r="AC65" s="5"/>
-    </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD65" s="20"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -8104,8 +8241,9 @@
       </c>
       <c r="AB66" s="5"/>
       <c r="AC66" s="5"/>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD66" s="20"/>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -8173,8 +8311,9 @@
         <v>11</v>
       </c>
       <c r="AC67" s="5"/>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD67" s="20"/>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -8242,8 +8381,9 @@
         <v>11</v>
       </c>
       <c r="AC68" s="5"/>
-    </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD68" s="20"/>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -8311,8 +8451,9 @@
         <v>11</v>
       </c>
       <c r="AC69" s="5"/>
-    </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD69" s="20"/>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -8380,8 +8521,9 @@
         <v>11</v>
       </c>
       <c r="AC70" s="5"/>
-    </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD70" s="20"/>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>185</v>
       </c>
@@ -8431,8 +8573,9 @@
         <v>11</v>
       </c>
       <c r="AC71" s="5"/>
-    </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD71" s="20"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -8498,8 +8641,9 @@
         <v>11</v>
       </c>
       <c r="AC72" s="5"/>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD72" s="20"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -8563,8 +8707,9 @@
       <c r="AA73" s="5"/>
       <c r="AB73" s="5"/>
       <c r="AC73" s="5"/>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD73" s="20"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -8626,8 +8771,9 @@
       <c r="AA74" s="5"/>
       <c r="AB74" s="5"/>
       <c r="AC74" s="5"/>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD74" s="20"/>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -8689,8 +8835,9 @@
         <v>11</v>
       </c>
       <c r="AC75" s="5"/>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD75" s="20"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -8758,8 +8905,9 @@
         <v>11</v>
       </c>
       <c r="AC76" s="5"/>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD76" s="20"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -8829,8 +8977,9 @@
         <v>11</v>
       </c>
       <c r="AC77" s="5"/>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD77" s="20"/>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -8898,8 +9047,9 @@
         <v>11</v>
       </c>
       <c r="AC78" s="5"/>
-    </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD78" s="20"/>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -8965,8 +9115,9 @@
         <v>11</v>
       </c>
       <c r="AC79" s="5"/>
-    </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD79" s="20"/>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -9030,8 +9181,9 @@
         <v>11</v>
       </c>
       <c r="AC80" s="5"/>
-    </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD80" s="20"/>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -9093,8 +9245,9 @@
         <v>11</v>
       </c>
       <c r="AC81" s="5"/>
-    </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD81" s="20"/>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -9158,8 +9311,9 @@
         <v>11</v>
       </c>
       <c r="AC82" s="5"/>
-    </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD82" s="20"/>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -9223,8 +9377,9 @@
       <c r="AA83" s="5"/>
       <c r="AB83" s="5"/>
       <c r="AC83" s="5"/>
-    </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD83" s="20"/>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -9290,8 +9445,9 @@
         <v>11</v>
       </c>
       <c r="AC84" s="5"/>
-    </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD84" s="20"/>
+    </row>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -9357,8 +9513,9 @@
         <v>11</v>
       </c>
       <c r="AC85" s="5"/>
-    </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD85" s="20"/>
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>218</v>
       </c>
@@ -9410,8 +9567,9 @@
         <v>11</v>
       </c>
       <c r="AC86" s="5"/>
-    </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD86" s="20"/>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -9475,8 +9633,9 @@
       <c r="AA87" s="5"/>
       <c r="AB87" s="5"/>
       <c r="AC87" s="5"/>
-    </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD87" s="20"/>
+    </row>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -9540,8 +9699,9 @@
       <c r="AA88" s="5"/>
       <c r="AB88" s="5"/>
       <c r="AC88" s="5"/>
-    </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD88" s="20"/>
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -9601,8 +9761,9 @@
       <c r="AA89" s="5"/>
       <c r="AB89" s="5"/>
       <c r="AC89" s="5"/>
-    </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD89" s="20"/>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -9664,8 +9825,9 @@
       </c>
       <c r="AB90" s="5"/>
       <c r="AC90" s="5"/>
-    </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD90" s="20"/>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -9727,8 +9889,9 @@
       <c r="AA91" s="5"/>
       <c r="AB91" s="5"/>
       <c r="AC91" s="5"/>
-    </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD91" s="20"/>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -9790,8 +9953,9 @@
       <c r="AA92" s="5"/>
       <c r="AB92" s="5"/>
       <c r="AC92" s="5"/>
-    </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD92" s="20"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -9851,8 +10015,9 @@
       <c r="AA93" s="5"/>
       <c r="AB93" s="5"/>
       <c r="AC93" s="5"/>
-    </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD93" s="20"/>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -9916,8 +10081,9 @@
         <v>11</v>
       </c>
       <c r="AC94" s="5"/>
-    </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD94" s="20"/>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -9981,8 +10147,9 @@
         <v>11</v>
       </c>
       <c r="AC95" s="5"/>
-    </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD95" s="20"/>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -10046,8 +10213,9 @@
         <v>11</v>
       </c>
       <c r="AC96" s="5"/>
-    </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD96" s="20"/>
+    </row>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -10111,8 +10279,9 @@
         <v>11</v>
       </c>
       <c r="AC97" s="5"/>
-    </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD97" s="20"/>
+    </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -10172,8 +10341,9 @@
       <c r="AA98" s="5"/>
       <c r="AB98" s="5"/>
       <c r="AC98" s="5"/>
-    </row>
-    <row r="99" spans="1:29" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="AD98" s="20"/>
+    </row>
+    <row r="99" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -10233,8 +10403,9 @@
       <c r="AA99" s="5"/>
       <c r="AB99" s="5"/>
       <c r="AC99" s="5"/>
-    </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD99" s="20"/>
+    </row>
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -10294,8 +10465,9 @@
       <c r="AA100" s="5"/>
       <c r="AB100" s="5"/>
       <c r="AC100" s="5"/>
-    </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD100" s="20"/>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -10355,8 +10527,9 @@
       <c r="AA101" s="5"/>
       <c r="AB101" s="5"/>
       <c r="AC101" s="5"/>
-    </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD101" s="20"/>
+    </row>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -10416,8 +10589,9 @@
       <c r="AA102" s="5"/>
       <c r="AB102" s="5"/>
       <c r="AC102" s="5"/>
-    </row>
-    <row r="103" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AD102" s="20"/>
+    </row>
+    <row r="103" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -10477,8 +10651,9 @@
       <c r="AA103" s="5"/>
       <c r="AB103" s="5"/>
       <c r="AC103" s="5"/>
-    </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD103" s="20"/>
+    </row>
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -10538,8 +10713,9 @@
       <c r="AA104" s="5"/>
       <c r="AB104" s="5"/>
       <c r="AC104" s="5"/>
-    </row>
-    <row r="105" spans="1:29" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AD104" s="20"/>
+    </row>
+    <row r="105" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -10599,8 +10775,9 @@
       <c r="AA105" s="5"/>
       <c r="AB105" s="5"/>
       <c r="AC105" s="5"/>
-    </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD105" s="20"/>
+    </row>
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -10662,8 +10839,9 @@
       <c r="AA106" s="5"/>
       <c r="AB106" s="5"/>
       <c r="AC106" s="5"/>
-    </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD106" s="20"/>
+    </row>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -10723,8 +10901,9 @@
       <c r="AA107" s="5"/>
       <c r="AB107" s="5"/>
       <c r="AC107" s="5"/>
-    </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD107" s="20"/>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -10786,8 +10965,9 @@
       <c r="AA108" s="5"/>
       <c r="AB108" s="5"/>
       <c r="AC108" s="5"/>
-    </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD108" s="20"/>
+    </row>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -10849,8 +11029,9 @@
       <c r="AA109" s="5"/>
       <c r="AB109" s="5"/>
       <c r="AC109" s="5"/>
-    </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD109" s="20"/>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -10910,8 +11091,9 @@
       <c r="AA110" s="5"/>
       <c r="AB110" s="5"/>
       <c r="AC110" s="5"/>
-    </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD110" s="20"/>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -10979,8 +11161,9 @@
         <v>11</v>
       </c>
       <c r="AC111" s="5"/>
-    </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD111" s="20"/>
+    </row>
+    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -11048,8 +11231,9 @@
         <v>11</v>
       </c>
       <c r="AC112" s="5"/>
-    </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD112" s="20"/>
+    </row>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>282</v>
       </c>
@@ -11099,8 +11283,9 @@
         <v>11</v>
       </c>
       <c r="AC113" s="5"/>
-    </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD113" s="20"/>
+    </row>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -11168,8 +11353,9 @@
         <v>11</v>
       </c>
       <c r="AC114" s="5"/>
-    </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD114" s="20"/>
+    </row>
+    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -11237,8 +11423,9 @@
         <v>11</v>
       </c>
       <c r="AC115" s="5"/>
-    </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD115" s="20"/>
+    </row>
+    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -11310,8 +11497,9 @@
         <v>11</v>
       </c>
       <c r="AC116" s="5"/>
-    </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD116" s="20"/>
+    </row>
+    <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -11377,8 +11565,9 @@
         <v>11</v>
       </c>
       <c r="AC117" s="5"/>
-    </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD117" s="20"/>
+    </row>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -11444,8 +11633,9 @@
         <v>11</v>
       </c>
       <c r="AC118" s="5"/>
-    </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD118" s="20"/>
+    </row>
+    <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -11513,8 +11703,9 @@
         <v>11</v>
       </c>
       <c r="AC119" s="5"/>
-    </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD119" s="20"/>
+    </row>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -11580,8 +11771,9 @@
         <v>11</v>
       </c>
       <c r="AC120" s="5"/>
-    </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD120" s="20"/>
+    </row>
+    <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -11647,8 +11839,9 @@
         <v>11</v>
       </c>
       <c r="AC121" s="5"/>
-    </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD121" s="20"/>
+    </row>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>304</v>
       </c>
@@ -11694,8 +11887,9 @@
         <v>11</v>
       </c>
       <c r="AC122" s="5"/>
-    </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD122" s="20"/>
+    </row>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -11755,8 +11949,9 @@
         <v>11</v>
       </c>
       <c r="AC123" s="5"/>
-    </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD123" s="20"/>
+    </row>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -11816,8 +12011,9 @@
         <v>11</v>
       </c>
       <c r="AC124" s="5"/>
-    </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD124" s="20"/>
+    </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -11877,8 +12073,9 @@
         <v>11</v>
       </c>
       <c r="AC125" s="5"/>
-    </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD125" s="20"/>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -11938,8 +12135,9 @@
         <v>11</v>
       </c>
       <c r="AC126" s="5"/>
-    </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD126" s="20"/>
+    </row>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -11999,8 +12197,9 @@
         <v>11</v>
       </c>
       <c r="AC127" s="5"/>
-    </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD127" s="20"/>
+    </row>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -12060,8 +12259,9 @@
         <v>11</v>
       </c>
       <c r="AC128" s="5"/>
-    </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD128" s="20"/>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -12121,8 +12321,9 @@
         <v>11</v>
       </c>
       <c r="AC129" s="5"/>
-    </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD129" s="20"/>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -12182,8 +12383,9 @@
         <v>11</v>
       </c>
       <c r="AC130" s="5"/>
-    </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD130" s="20"/>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -12243,8 +12445,9 @@
         <v>11</v>
       </c>
       <c r="AC131" s="5"/>
-    </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD131" s="20"/>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -12304,8 +12507,9 @@
         <v>11</v>
       </c>
       <c r="AC132" s="5"/>
-    </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD132" s="20"/>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -12363,8 +12567,9 @@
       <c r="AA133" s="5"/>
       <c r="AB133" s="5"/>
       <c r="AC133" s="5"/>
-    </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD133" s="20"/>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -12422,8 +12627,9 @@
       <c r="AA134" s="5"/>
       <c r="AB134" s="5"/>
       <c r="AC134" s="5"/>
-    </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD134" s="20"/>
+    </row>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -12481,8 +12687,9 @@
       <c r="AA135" s="5"/>
       <c r="AB135" s="5"/>
       <c r="AC135" s="5"/>
-    </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD135" s="20"/>
+    </row>
+    <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -12540,8 +12747,9 @@
       <c r="AA136" s="5"/>
       <c r="AB136" s="5"/>
       <c r="AC136" s="5"/>
-    </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD136" s="20"/>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -12599,8 +12807,9 @@
       <c r="AA137" s="5"/>
       <c r="AB137" s="5"/>
       <c r="AC137" s="5"/>
-    </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD137" s="20"/>
+    </row>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -12660,8 +12869,9 @@
         <v>11</v>
       </c>
       <c r="AC138" s="5"/>
-    </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD138" s="20"/>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -12721,8 +12931,9 @@
         <v>11</v>
       </c>
       <c r="AC139" s="5"/>
-    </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD139" s="20"/>
+    </row>
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -12782,8 +12993,9 @@
         <v>11</v>
       </c>
       <c r="AC140" s="5"/>
-    </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD140" s="20"/>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -12843,8 +13055,9 @@
         <v>11</v>
       </c>
       <c r="AC141" s="5"/>
-    </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD141" s="20"/>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -12904,8 +13117,9 @@
         <v>11</v>
       </c>
       <c r="AC142" s="5"/>
-    </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD142" s="20"/>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -12965,8 +13179,9 @@
         <v>11</v>
       </c>
       <c r="AC143" s="5"/>
-    </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD143" s="20"/>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -13026,8 +13241,9 @@
         <v>11</v>
       </c>
       <c r="AC144" s="5"/>
-    </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD144" s="20"/>
+    </row>
+    <row r="145" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -13089,8 +13305,9 @@
         <v>11</v>
       </c>
       <c r="AC145" s="5"/>
-    </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD145" s="20"/>
+    </row>
+    <row r="146" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -13152,8 +13369,9 @@
         <v>11</v>
       </c>
       <c r="AC146" s="5"/>
-    </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD146" s="20"/>
+    </row>
+    <row r="147" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -13217,8 +13435,9 @@
       </c>
       <c r="AB147" s="5"/>
       <c r="AC147" s="5"/>
-    </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD147" s="20"/>
+    </row>
+    <row r="148" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -13278,8 +13497,9 @@
         <v>11</v>
       </c>
       <c r="AC148" s="5"/>
-    </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD148" s="20"/>
+    </row>
+    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -13339,8 +13559,9 @@
         <v>11</v>
       </c>
       <c r="AC149" s="5"/>
-    </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD149" s="20"/>
+    </row>
+    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>368</v>
       </c>
@@ -13384,8 +13605,9 @@
         <v>23</v>
       </c>
       <c r="AC150" s="5"/>
-    </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD150" s="20"/>
+    </row>
+    <row r="151" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -13445,8 +13667,9 @@
         <v>23</v>
       </c>
       <c r="AC151" s="5"/>
-    </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD151" s="20"/>
+    </row>
+    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -13506,8 +13729,9 @@
         <v>23</v>
       </c>
       <c r="AC152" s="5"/>
-    </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD152" s="20"/>
+    </row>
+    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -13567,8 +13791,9 @@
         <v>23</v>
       </c>
       <c r="AC153" s="5"/>
-    </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD153" s="20"/>
+    </row>
+    <row r="154" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -13628,8 +13853,9 @@
         <v>23</v>
       </c>
       <c r="AC154" s="5"/>
-    </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD154" s="20"/>
+    </row>
+    <row r="155" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -13689,8 +13915,9 @@
         <v>23</v>
       </c>
       <c r="AC155" s="5"/>
-    </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD155" s="20"/>
+    </row>
+    <row r="156" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -13748,8 +13975,9 @@
         <v>23</v>
       </c>
       <c r="AC156" s="5"/>
-    </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD156" s="20"/>
+    </row>
+    <row r="157" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>384</v>
       </c>
@@ -13793,8 +14021,9 @@
         <v>23</v>
       </c>
       <c r="AC157" s="5"/>
-    </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD157" s="20"/>
+    </row>
+    <row r="158" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -13856,8 +14085,9 @@
         <v>23</v>
       </c>
       <c r="AC158" s="5"/>
-    </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD158" s="20"/>
+    </row>
+    <row r="159" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -13919,8 +14149,9 @@
         <v>23</v>
       </c>
       <c r="AC159" s="5"/>
-    </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD159" s="20"/>
+    </row>
+    <row r="160" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -13982,8 +14213,9 @@
         <v>23</v>
       </c>
       <c r="AC160" s="5"/>
-    </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD160" s="20"/>
+    </row>
+    <row r="161" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -14045,8 +14277,9 @@
         <v>23</v>
       </c>
       <c r="AC161" s="5"/>
-    </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD161" s="20"/>
+    </row>
+    <row r="162" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -14108,8 +14341,9 @@
         <v>23</v>
       </c>
       <c r="AC162" s="5"/>
-    </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD162" s="20"/>
+    </row>
+    <row r="163" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -14171,8 +14405,9 @@
         <v>23</v>
       </c>
       <c r="AC163" s="5"/>
-    </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD163" s="20"/>
+    </row>
+    <row r="164" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -14234,8 +14469,9 @@
         <v>23</v>
       </c>
       <c r="AC164" s="5"/>
-    </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD164" s="20"/>
+    </row>
+    <row r="165" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -14297,8 +14533,9 @@
         <v>23</v>
       </c>
       <c r="AC165" s="5"/>
-    </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD165" s="20"/>
+    </row>
+    <row r="166" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -14360,8 +14597,9 @@
         <v>23</v>
       </c>
       <c r="AC166" s="5"/>
-    </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD166" s="20"/>
+    </row>
+    <row r="167" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -14423,8 +14661,9 @@
         <v>23</v>
       </c>
       <c r="AC167" s="5"/>
-    </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD167" s="20"/>
+    </row>
+    <row r="168" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -14486,8 +14725,9 @@
         <v>23</v>
       </c>
       <c r="AC168" s="5"/>
-    </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD168" s="20"/>
+    </row>
+    <row r="169" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -14549,8 +14789,9 @@
         <v>23</v>
       </c>
       <c r="AC169" s="5"/>
-    </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD169" s="20"/>
+    </row>
+    <row r="170" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -14612,8 +14853,9 @@
         <v>23</v>
       </c>
       <c r="AC170" s="5"/>
-    </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD170" s="20"/>
+    </row>
+    <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -14677,8 +14919,9 @@
         <v>23</v>
       </c>
       <c r="AC171" s="5"/>
-    </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD171" s="20"/>
+    </row>
+    <row r="172" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -14738,8 +14981,9 @@
         <v>23</v>
       </c>
       <c r="AC172" s="5"/>
-    </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD172" s="20"/>
+    </row>
+    <row r="173" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -14797,8 +15041,9 @@
         <v>23</v>
       </c>
       <c r="AC173" s="5"/>
-    </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD173" s="20"/>
+    </row>
+    <row r="174" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>424</v>
       </c>
@@ -14854,8 +15099,9 @@
       <c r="AC174" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD174" s="20"/>
+    </row>
+    <row r="175" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -14927,8 +15173,9 @@
         <v>11</v>
       </c>
       <c r="AC175" s="5"/>
-    </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD175" s="20"/>
+    </row>
+    <row r="176" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -14994,8 +15241,9 @@
         <v>11</v>
       </c>
       <c r="AC176" s="5"/>
-    </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD176" s="20"/>
+    </row>
+    <row r="177" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -15067,8 +15315,9 @@
       <c r="AC177" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD177" s="20"/>
+    </row>
+    <row r="178" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -15140,8 +15389,9 @@
         <v>11</v>
       </c>
       <c r="AC178" s="5"/>
-    </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD178" s="20"/>
+    </row>
+    <row r="179" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -15215,8 +15465,9 @@
         <v>11</v>
       </c>
       <c r="AC179" s="5"/>
-    </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD179" s="20"/>
+    </row>
+    <row r="180" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -15286,8 +15537,9 @@
         <v>11</v>
       </c>
       <c r="AC180" s="5"/>
-    </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD180" s="20"/>
+    </row>
+    <row r="181" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -15355,8 +15607,9 @@
         <v>11</v>
       </c>
       <c r="AC181" s="5"/>
-    </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD181" s="20"/>
+    </row>
+    <row r="182" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>447</v>
       </c>
@@ -15406,8 +15659,9 @@
         <v>11</v>
       </c>
       <c r="AC182" s="5"/>
-    </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD182" s="20"/>
+    </row>
+    <row r="183" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -15469,8 +15723,9 @@
       <c r="AA183" s="5"/>
       <c r="AB183" s="5"/>
       <c r="AC183" s="5"/>
-    </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD183" s="20"/>
+    </row>
+    <row r="184" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -15534,8 +15789,9 @@
         <v>11</v>
       </c>
       <c r="AC184" s="5"/>
-    </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD184" s="20"/>
+    </row>
+    <row r="185" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -15595,8 +15851,9 @@
       <c r="AA185" s="5"/>
       <c r="AB185" s="5"/>
       <c r="AC185" s="5"/>
-    </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD185" s="20"/>
+    </row>
+    <row r="186" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -15658,8 +15915,9 @@
       <c r="AA186" s="6"/>
       <c r="AB186" s="6"/>
       <c r="AC186" s="6"/>
-    </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD186" s="20"/>
+    </row>
+    <row r="187" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -15721,8 +15979,9 @@
       <c r="AA187" s="6"/>
       <c r="AB187" s="6"/>
       <c r="AC187" s="6"/>
-    </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD187" s="20"/>
+    </row>
+    <row r="188" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -15786,8 +16045,9 @@
         <v>11</v>
       </c>
       <c r="AC188" s="6"/>
-    </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD188" s="20"/>
+    </row>
+    <row r="189" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -15847,8 +16107,9 @@
       <c r="AA189" s="6"/>
       <c r="AB189" s="6"/>
       <c r="AC189" s="6"/>
-    </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD189" s="20"/>
+    </row>
+    <row r="190" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -15910,8 +16171,9 @@
       <c r="AA190" s="6"/>
       <c r="AB190" s="6"/>
       <c r="AC190" s="6"/>
-    </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD190" s="20"/>
+    </row>
+    <row r="191" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -15973,8 +16235,9 @@
       <c r="AA191" s="6"/>
       <c r="AB191" s="6"/>
       <c r="AC191" s="6"/>
-    </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD191" s="20"/>
+    </row>
+    <row r="192" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -16036,8 +16299,9 @@
       <c r="AA192" s="6"/>
       <c r="AB192" s="6"/>
       <c r="AC192" s="6"/>
-    </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD192" s="20"/>
+    </row>
+    <row r="193" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -16099,8 +16363,9 @@
       </c>
       <c r="AB193" s="6"/>
       <c r="AC193" s="6"/>
-    </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD193" s="20"/>
+    </row>
+    <row r="194" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -16162,8 +16427,9 @@
       </c>
       <c r="AB194" s="6"/>
       <c r="AC194" s="6"/>
-    </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD194" s="20"/>
+    </row>
+    <row r="195" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -16227,8 +16493,9 @@
       <c r="AA195" s="6"/>
       <c r="AB195" s="6"/>
       <c r="AC195" s="6"/>
-    </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD195" s="20"/>
+    </row>
+    <row r="196" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -16292,8 +16559,9 @@
       <c r="AA196" s="6"/>
       <c r="AB196" s="6"/>
       <c r="AC196" s="6"/>
-    </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD196" s="20"/>
+    </row>
+    <row r="197" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -16355,8 +16623,9 @@
       <c r="AA197" s="6"/>
       <c r="AB197" s="6"/>
       <c r="AC197" s="6"/>
-    </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD197" s="20"/>
+    </row>
+    <row r="198" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -16422,8 +16691,9 @@
         <v>11</v>
       </c>
       <c r="AC198" s="6"/>
-    </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD198" s="20"/>
+    </row>
+    <row r="199" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -16489,8 +16759,9 @@
         <v>11</v>
       </c>
       <c r="AC199" s="6"/>
-    </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD199" s="20"/>
+    </row>
+    <row r="200" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>494</v>
       </c>
@@ -16536,8 +16807,9 @@
       </c>
       <c r="AB200" s="6"/>
       <c r="AC200" s="6"/>
-    </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD200" s="20"/>
+    </row>
+    <row r="201" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -16597,8 +16869,9 @@
       </c>
       <c r="AB201" s="6"/>
       <c r="AC201" s="6"/>
-    </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD201" s="20"/>
+    </row>
+    <row r="202" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -16662,8 +16935,9 @@
       </c>
       <c r="AB202" s="6"/>
       <c r="AC202" s="6"/>
-    </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD202" s="20"/>
+    </row>
+    <row r="203" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -16729,8 +17003,9 @@
       </c>
       <c r="AB203" s="6"/>
       <c r="AC203" s="6"/>
-    </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD203" s="20"/>
+    </row>
+    <row r="204" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>501</v>
       </c>
@@ -16782,8 +17057,9 @@
         <v>11</v>
       </c>
       <c r="AC204" s="6"/>
-    </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD204" s="20"/>
+    </row>
+    <row r="205" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -16853,8 +17129,9 @@
         <v>11</v>
       </c>
       <c r="AC205" s="6"/>
-    </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD205" s="20"/>
+    </row>
+    <row r="206" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -16920,8 +17197,9 @@
         <v>11</v>
       </c>
       <c r="AC206" s="6"/>
-    </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD206" s="20"/>
+    </row>
+    <row r="207" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -16987,8 +17265,9 @@
       </c>
       <c r="AB207" s="6"/>
       <c r="AC207" s="6"/>
-    </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD207" s="20"/>
+    </row>
+    <row r="208" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -17054,8 +17333,9 @@
       </c>
       <c r="AB208" s="6"/>
       <c r="AC208" s="6"/>
-    </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD208" s="20"/>
+    </row>
+    <row r="209" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -17121,8 +17401,9 @@
         <v>11</v>
       </c>
       <c r="AC209" s="6"/>
-    </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD209" s="20"/>
+    </row>
+    <row r="210" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -17188,8 +17469,9 @@
       </c>
       <c r="AB210" s="6"/>
       <c r="AC210" s="6"/>
-    </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD210" s="20"/>
+    </row>
+    <row r="211" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -17251,8 +17533,9 @@
       <c r="AA211" s="6"/>
       <c r="AB211" s="6"/>
       <c r="AC211" s="6"/>
-    </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD211" s="20"/>
+    </row>
+    <row r="212" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>525</v>
       </c>
@@ -17298,8 +17581,9 @@
       <c r="AA212" s="6"/>
       <c r="AB212" s="6"/>
       <c r="AC212" s="6"/>
-    </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD212" s="20"/>
+    </row>
+    <row r="213" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -17361,8 +17645,9 @@
       <c r="AA213" s="6"/>
       <c r="AB213" s="6"/>
       <c r="AC213" s="6"/>
-    </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD213" s="20"/>
+    </row>
+    <row r="214" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -17424,8 +17709,9 @@
       <c r="AA214" s="6"/>
       <c r="AB214" s="6"/>
       <c r="AC214" s="6"/>
-    </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD214" s="20"/>
+    </row>
+    <row r="215" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>0</v>
       </c>
@@ -17469,8 +17755,9 @@
       <c r="AA215" s="6"/>
       <c r="AB215" s="6"/>
       <c r="AC215" s="6"/>
-    </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD215" s="20"/>
+    </row>
+    <row r="216" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -17532,8 +17819,9 @@
       <c r="AA216" s="6"/>
       <c r="AB216" s="6"/>
       <c r="AC216" s="6"/>
-    </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD216" s="20"/>
+    </row>
+    <row r="217" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>534</v>
       </c>
@@ -17583,8 +17871,9 @@
       <c r="AC217" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD217" s="20"/>
+    </row>
+    <row r="218" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -17650,8 +17939,9 @@
       <c r="AC218" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD218" s="20"/>
+    </row>
+    <row r="219" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>2</v>
       </c>
@@ -17693,8 +17983,9 @@
       <c r="AC219" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD219" s="20"/>
+    </row>
+    <row r="220" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -17752,8 +18043,9 @@
       <c r="AC220" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD220" s="20"/>
+    </row>
+    <row r="221" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>542</v>
       </c>
@@ -17795,8 +18087,9 @@
       <c r="AC221" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD221" s="20"/>
+    </row>
+    <row r="222" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -17854,8 +18147,9 @@
       <c r="AC222" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD222" s="20"/>
+    </row>
+    <row r="223" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>1</v>
       </c>
@@ -17897,8 +18191,9 @@
       <c r="AA223" s="6"/>
       <c r="AB223" s="6"/>
       <c r="AC223" s="6"/>
-    </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD223" s="20"/>
+    </row>
+    <row r="224" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -17958,19 +18253,28 @@
       <c r="AA224" s="6"/>
       <c r="AB224" s="6"/>
       <c r="AC224" s="6"/>
+      <c r="AD224" s="20"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:AC224"/>
   <conditionalFormatting sqref="V1:AC1">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
       <formula>"r"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:AC224">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"s"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"r"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD1">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>

</xml_diff>